<commit_message>
tidied up the population ordering
</commit_message>
<xml_diff>
--- a/pop_names.xlsx
+++ b/pop_names.xlsx
@@ -15,7 +15,10 @@
     <sheet name="pop_names" sheetId="1" r:id="rId1"/>
     <sheet name="Colors" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pop_names!$A$1:$E$29</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>Code</t>
   </si>
@@ -271,6 +274,9 @@
   </si>
   <si>
     <t>Middle-east Wolf</t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
@@ -585,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,7 +603,7 @@
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,8 +616,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -625,43 +634,55 @@
         <f>VLOOKUP(C2,Colors!A:B,2,FALSE)</f>
         <v>#a6cee3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f>VLOOKUP(D2,Colors!B:C,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="str">
         <f>VLOOKUP(C3,Colors!A:B,2,FALSE)</f>
-        <v>#1f78b4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#a6cee3</v>
+      </c>
+      <c r="E3">
+        <f>VLOOKUP(D3,Colors!B:C,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" t="str">
         <f>VLOOKUP(C4,Colors!A:B,2,FALSE)</f>
-        <v>#b2df8a</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#33a02c</v>
+      </c>
+      <c r="E4">
+        <f>VLOOKUP(D4,Colors!B:C,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -670,53 +691,69 @@
         <f>VLOOKUP(C5,Colors!A:B,2,FALSE)</f>
         <v>#33a02c</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f>VLOOKUP(D5,Colors!B:C,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" t="str">
         <f>VLOOKUP(C6,Colors!A:B,2,FALSE)</f>
-        <v>#fb9a99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#33a02c</v>
+      </c>
+      <c r="E6">
+        <f>VLOOKUP(D6,Colors!B:C,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7" t="str">
         <f>VLOOKUP(C7,Colors!A:B,2,FALSE)</f>
-        <v>#e31a1c</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#33a02c</v>
+      </c>
+      <c r="E7">
+        <f>VLOOKUP(D7,Colors!B:C,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D8" t="str">
         <f>VLOOKUP(C8,Colors!A:B,2,FALSE)</f>
-        <v>#33a02c</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#fb9a99</v>
+      </c>
+      <c r="E8">
+        <f>VLOOKUP(D8,Colors!B:C,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -730,28 +767,36 @@
         <f>VLOOKUP(C9,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <f>VLOOKUP(D9,Colors!B:C,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D10" t="str">
         <f>VLOOKUP(C10,Colors!A:B,2,FALSE)</f>
-        <v>#33a02c</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#fb9a99</v>
+      </c>
+      <c r="E10">
+        <f>VLOOKUP(D10,Colors!B:C,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -760,238 +805,302 @@
         <f>VLOOKUP(C11,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <f>VLOOKUP(D11,Colors!B:C,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D12" t="str">
         <f>VLOOKUP(C12,Colors!A:B,2,FALSE)</f>
-        <v>#fdbf6f</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#fb9a99</v>
+      </c>
+      <c r="E12">
+        <f>VLOOKUP(D12,Colors!B:C,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D13" t="str">
         <f>VLOOKUP(C13,Colors!A:B,2,FALSE)</f>
-        <v>#ff7f00</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#cab2d6</v>
+      </c>
+      <c r="E13">
+        <f>VLOOKUP(D13,Colors!B:C,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D14" t="str">
         <f>VLOOKUP(C14,Colors!A:B,2,FALSE)</f>
-        <v>#33a02c</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#cab2d6</v>
+      </c>
+      <c r="E14">
+        <f>VLOOKUP(D14,Colors!B:C,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D15" t="str">
         <f>VLOOKUP(C15,Colors!A:B,2,FALSE)</f>
-        <v>#fb9a99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#fdbf6f</v>
+      </c>
+      <c r="E15">
+        <f>VLOOKUP(D15,Colors!B:C,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D16" t="str">
         <f>VLOOKUP(C16,Colors!A:B,2,FALSE)</f>
-        <v>#cab2d6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#fdbf6f</v>
+      </c>
+      <c r="E16">
+        <f>VLOOKUP(D16,Colors!B:C,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D17" t="str">
         <f>VLOOKUP(C17,Colors!A:B,2,FALSE)</f>
-        <v>#a6cee3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#e31a1c</v>
+      </c>
+      <c r="E17">
+        <f>VLOOKUP(D17,Colors!B:C,2,FALSE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D18" t="str">
         <f>VLOOKUP(C18,Colors!A:B,2,FALSE)</f>
-        <v>#6a3d9a</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#e31a1c</v>
+      </c>
+      <c r="E18">
+        <f>VLOOKUP(D18,Colors!B:C,2,FALSE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D19" t="str">
         <f>VLOOKUP(C19,Colors!A:B,2,FALSE)</f>
-        <v>#cab2d6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#e31a1c</v>
+      </c>
+      <c r="E19">
+        <f>VLOOKUP(D19,Colors!B:C,2,FALSE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D20" t="str">
         <f>VLOOKUP(C20,Colors!A:B,2,FALSE)</f>
-        <v>#fdbf6f</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#e31a1c</v>
+      </c>
+      <c r="E20">
+        <f>VLOOKUP(D20,Colors!B:C,2,FALSE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D21" t="str">
         <f>VLOOKUP(C21,Colors!A:B,2,FALSE)</f>
-        <v>#fb9a99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#6a3d9a</v>
+      </c>
+      <c r="E21">
+        <f>VLOOKUP(D21,Colors!B:C,2,FALSE)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D22" t="str">
         <f>VLOOKUP(C22,Colors!A:B,2,FALSE)</f>
-        <v>#e31a1c</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#b2df8a</v>
+      </c>
+      <c r="E22">
+        <f>VLOOKUP(D22,Colors!B:C,2,FALSE)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D23" t="str">
         <f>VLOOKUP(C23,Colors!A:B,2,FALSE)</f>
-        <v>#e31a1c</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#ff7f00</v>
+      </c>
+      <c r="E23">
+        <f>VLOOKUP(D23,Colors!B:C,2,FALSE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D24" t="str">
         <f>VLOOKUP(C24,Colors!A:B,2,FALSE)</f>
-        <v>#e31a1c</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#1f78b4</v>
+      </c>
+      <c r="E24">
+        <f>VLOOKUP(D24,Colors!B:C,2,FALSE)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D25" t="str">
         <f>VLOOKUP(C25,Colors!A:B,2,FALSE)</f>
-        <v>#ffff99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#b15928</v>
+      </c>
+      <c r="E25">
+        <f>VLOOKUP(D25,Colors!B:C,2,FALSE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D26" t="str">
         <f>VLOOKUP(C26,Colors!A:B,2,FALSE)</f>
-        <v>#b15928</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>#003c30</v>
+      </c>
+      <c r="E26">
+        <f>VLOOKUP(D26,Colors!B:C,2,FALSE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
         <v>75</v>
@@ -1000,13 +1109,17 @@
         <f>VLOOKUP(C27,Colors!A:B,2,FALSE)</f>
         <v>#003c30</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <f>VLOOKUP(D27,Colors!B:C,2,FALSE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
         <v>75</v>
@@ -1015,33 +1128,47 @@
         <f>VLOOKUP(C28,Colors!A:B,2,FALSE)</f>
         <v>#003c30</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <f>VLOOKUP(D28,Colors!B:C,2,FALSE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D29" t="str">
         <f>VLOOKUP(C29,Colors!A:B,2,FALSE)</f>
-        <v>#003c30</v>
+        <v>#ffff99</v>
+      </c>
+      <c r="E29">
+        <f>VLOOKUP(D29,Colors!B:C,2,FALSE)</f>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E29">
+    <sortState ref="A2:E29">
+      <sortCondition ref="E2:E29"/>
+      <sortCondition ref="A2:A29"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,108 +1176,147 @@
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" t="s">
-        <v>76</v>
+      <c r="C13">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidied up NJ tree plotting
</commit_message>
<xml_diff>
--- a/pop_names.xlsx
+++ b/pop_names.xlsx
@@ -240,9 +240,6 @@
     <t>Outgroup</t>
   </si>
   <si>
-    <t>#ffff99</t>
-  </si>
-  <si>
     <t>WAM</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>#4d4d4d</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +617,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1059,13 +1059,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="str">
         <f>VLOOKUP(C25,Colors!A:B,2,FALSE)</f>
@@ -1078,13 +1078,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
       </c>
       <c r="D26" t="str">
         <f>VLOOKUP(C26,Colors!A:B,2,FALSE)</f>
@@ -1097,13 +1097,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" t="str">
         <f>VLOOKUP(C27,Colors!A:B,2,FALSE)</f>
@@ -1116,13 +1116,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" t="str">
         <f>VLOOKUP(C28,Colors!A:B,2,FALSE)</f>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="D29" t="str">
         <f>VLOOKUP(C29,Colors!A:B,2,FALSE)</f>
-        <v>#ffff99</v>
+        <v>#4d4d4d</v>
       </c>
       <c r="E29">
         <f>VLOOKUP(D29,Colors!B:C,2,FALSE)</f>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
         <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -1299,10 +1299,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
         <v>75</v>
-      </c>
-      <c r="B12" t="s">
-        <v>76</v>
       </c>
       <c r="C12">
         <v>12</v>
@@ -1313,7 +1313,7 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C13">
         <v>13</v>

</xml_diff>

<commit_message>
truncated overly long population/sample names
</commit_message>
<xml_diff>
--- a/pop_names.xlsx
+++ b/pop_names.xlsx
@@ -14,9 +14,11 @@
   <sheets>
     <sheet name="pop_names" sheetId="1" r:id="rId1"/>
     <sheet name="Colors" sheetId="2" r:id="rId2"/>
+    <sheet name="Truncated Names" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pop_names!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Truncated Names'!$A$1:$B$52</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="238">
   <si>
     <t>Code</t>
   </si>
@@ -433,6 +435,318 @@
   </si>
   <si>
     <t>#ae017e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alaskan_Malamute </t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American_Eskimo_Dog </t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American_Pit_Bull_Terrier </t>
+  </si>
+  <si>
+    <t>APBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American_Staffordshire_Terrier </t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basenji </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beagle </t>
+  </si>
+  <si>
+    <t>BEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boxer </t>
+  </si>
+  <si>
+    <t>BOX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carolina_Dog </t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catahoula_Leopard_Dog </t>
+  </si>
+  <si>
+    <t>CLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chesapeake_Bay_Retriever </t>
+  </si>
+  <si>
+    <t>CBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chihuahua </t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese_Shar-pei </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chow_Chow </t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eurasier </t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finnish_Spitz </t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greenland_Sledge_Dog </t>
+  </si>
+  <si>
+    <t>GSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New_Guinea_Singing_Dog </t>
+  </si>
+  <si>
+    <t>NGSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newfoundland </t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nova_Scotia_Duck_Tolling_Retriever </t>
+  </si>
+  <si>
+    <t>NSDTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peruvian_Inca_Orchid </t>
+  </si>
+  <si>
+    <t>PIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samoyed </t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siberian_Husky </t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taimyr </t>
+  </si>
+  <si>
+    <t>TAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Belize </t>
+  </si>
+  <si>
+    <t>VDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Brazil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Colombia </t>
+  </si>
+  <si>
+    <t>VDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Costa_Rica </t>
+  </si>
+  <si>
+    <t>VDCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Dominican_Republic </t>
+  </si>
+  <si>
+    <t>VDDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Honduras </t>
+  </si>
+  <si>
+    <t>VDH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_India-Chennai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_India-Dehli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_India-Hazaribagh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_India-Mumbai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_India-Orissa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Indonesia-Borneo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Indonesia-Jakarta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Panama </t>
+  </si>
+  <si>
+    <t>VDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Papua_New_Guinea-East_Highlands_ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Papua_New_Guinea-Port_Moresby </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Peru-Arequipa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Peru-Cusco </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Peru-Ica </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Peru-Loreto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Peru-Puno </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Puerto_Rico </t>
+  </si>
+  <si>
+    <t>VDPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_US-Alaska </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Vietnam-Cao_Bang </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Vietnam-Ha_Giang </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Vietnam-Lang_Son </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village_Dog_Vietnam-Lao_Cai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xoloitzcuintli </t>
+  </si>
+  <si>
+    <t>XOL</t>
+  </si>
+  <si>
+    <t>VDID</t>
+  </si>
+  <si>
+    <t>VDB2</t>
+  </si>
+  <si>
+    <t>BAS2</t>
+  </si>
+  <si>
+    <t>VDPNGPM</t>
+  </si>
+  <si>
+    <t>VDPA</t>
+  </si>
+  <si>
+    <t>VDVLC</t>
+  </si>
+  <si>
+    <t>VDVCB</t>
+  </si>
+  <si>
+    <t>VDIJ</t>
+  </si>
+  <si>
+    <t>VDPL</t>
+  </si>
+  <si>
+    <t>VDPP</t>
+  </si>
+  <si>
+    <t>VDPC</t>
+  </si>
+  <si>
+    <t>VDPI</t>
+  </si>
+  <si>
+    <t>VDIO</t>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>VDPNGEH</t>
+  </si>
+  <si>
+    <t>VDIM</t>
+  </si>
+  <si>
+    <t>VDIH</t>
+  </si>
+  <si>
+    <t>VDVLS</t>
+  </si>
+  <si>
+    <t>VDVHG</t>
+  </si>
+  <si>
+    <t>VDIB</t>
+  </si>
+  <si>
+    <t>VDIC</t>
+  </si>
+  <si>
+    <t>VDUA</t>
+  </si>
+  <si>
+    <t>Long Name</t>
+  </si>
+  <si>
+    <t>Short Name</t>
   </si>
 </sst>
 </file>
@@ -770,11 +1084,12 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -817,7 +1132,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -855,7 +1170,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
         <v>91</v>
@@ -874,7 +1189,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
         <v>92</v>
@@ -969,7 +1284,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
         <v>87</v>
@@ -1083,7 +1398,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
         <v>99</v>
@@ -1102,7 +1417,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
         <v>100</v>
@@ -1121,7 +1436,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
         <v>101</v>
@@ -1140,7 +1455,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
         <v>107</v>
@@ -1159,7 +1474,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
         <v>108</v>
@@ -1178,7 +1493,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
         <v>88</v>
@@ -1197,7 +1512,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
         <v>89</v>
@@ -1216,7 +1531,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
         <v>90</v>
@@ -1235,7 +1550,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
         <v>93</v>
@@ -1254,7 +1569,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
         <v>94</v>
@@ -1273,7 +1588,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
         <v>95</v>
@@ -1292,7 +1607,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>96</v>
@@ -1349,7 +1664,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
         <v>104</v>
@@ -1368,7 +1683,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -1387,7 +1702,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
         <v>106</v>
@@ -1406,7 +1721,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s">
         <v>109</v>
@@ -1425,7 +1740,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>215</v>
       </c>
       <c r="B35" t="s">
         <v>110</v>
@@ -1444,7 +1759,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="B36" t="s">
         <v>111</v>
@@ -1463,7 +1778,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
         <v>112</v>
@@ -1482,7 +1797,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="B38" t="s">
         <v>113</v>
@@ -1501,7 +1816,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
         <v>114</v>
@@ -1520,7 +1835,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="B40" t="s">
         <v>117</v>
@@ -1539,7 +1854,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>218</v>
       </c>
       <c r="B41" t="s">
         <v>120</v>
@@ -1558,7 +1873,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>224</v>
       </c>
       <c r="B42" t="s">
         <v>121</v>
@@ -1577,7 +1892,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>225</v>
       </c>
       <c r="B43" t="s">
         <v>122</v>
@@ -1596,7 +1911,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="B44" t="s">
         <v>123</v>
@@ -1615,7 +1930,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
       <c r="B45" t="s">
         <v>124</v>
@@ -1634,7 +1949,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>125</v>
+        <v>206</v>
       </c>
       <c r="B46" t="s">
         <v>125</v>
@@ -1653,7 +1968,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s">
         <v>126</v>
@@ -1672,7 +1987,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>213</v>
       </c>
       <c r="B48" t="s">
         <v>102</v>
@@ -1729,7 +2044,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>234</v>
       </c>
       <c r="B51" t="s">
         <v>82</v>
@@ -1748,7 +2063,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>214</v>
       </c>
       <c r="B52" t="s">
         <v>83</v>
@@ -1767,7 +2082,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>230</v>
       </c>
       <c r="B53" t="s">
         <v>84</v>
@@ -1786,7 +2101,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>229</v>
       </c>
       <c r="B54" t="s">
         <v>85</v>
@@ -1805,7 +2120,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>226</v>
       </c>
       <c r="B55" t="s">
         <v>86</v>
@@ -1824,7 +2139,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>227</v>
       </c>
       <c r="B56" t="s">
         <v>97</v>
@@ -1843,7 +2158,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
         <v>98</v>
@@ -1938,7 +2253,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
@@ -1957,7 +2272,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>115</v>
+        <v>233</v>
       </c>
       <c r="B63" t="s">
         <v>115</v>
@@ -1976,7 +2291,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="B64" t="s">
         <v>116</v>
@@ -1995,7 +2310,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>118</v>
+        <v>228</v>
       </c>
       <c r="B65" t="s">
         <v>118</v>
@@ -2014,7 +2329,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="B66" t="s">
         <v>119</v>
@@ -2033,7 +2348,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>220</v>
       </c>
       <c r="B67" t="s">
         <v>127</v>
@@ -2052,7 +2367,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>232</v>
       </c>
       <c r="B68" t="s">
         <v>128</v>
@@ -2071,7 +2386,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>231</v>
       </c>
       <c r="B69" t="s">
         <v>129</v>
@@ -2090,7 +2405,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>219</v>
       </c>
       <c r="B70" t="s">
         <v>130</v>
@@ -2261,7 +2576,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="B79" t="s">
         <v>131</v>
@@ -2482,4 +2797,444 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>194</v>
+      </c>
+      <c r="B36" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>204</v>
+      </c>
+      <c r="B45" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>205</v>
+      </c>
+      <c r="B46" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>209</v>
+      </c>
+      <c r="B49" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>210</v>
+      </c>
+      <c r="B50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B52">
+    <sortState ref="A2:B52">
+      <sortCondition ref="A1:A52"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
shapes now read from csv
</commit_message>
<xml_diff>
--- a/pop_names.xlsx
+++ b/pop_names.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,7 +17,7 @@
     <sheet name="Truncated Names" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pop_names!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pop_names!$A$1:$F$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Truncated Names'!$A$1:$B$52</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="239">
   <si>
     <t>Code</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t>Short Name</t>
+  </si>
+  <si>
+    <t>Shape</t>
   </si>
 </sst>
 </file>
@@ -1081,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1094,7 +1097,7 @@
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1108,10 +1111,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1126,11 +1132,15 @@
         <v>#a6cee3</v>
       </c>
       <c r="E2">
-        <f>VLOOKUP(C2,Colors!A:C,3,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D2,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <f>VLOOKUP(E2,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>216</v>
       </c>
@@ -1145,11 +1155,15 @@
         <v>#a6cee3</v>
       </c>
       <c r="E3">
-        <f>VLOOKUP(C3,Colors!A:C,3,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D3,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <f>VLOOKUP(E3,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1164,11 +1178,15 @@
         <v>#a6cee3</v>
       </c>
       <c r="E4">
-        <f>VLOOKUP(C4,Colors!A:C,3,FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D4,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <f>VLOOKUP(E4,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -1183,11 +1201,15 @@
         <v>#33a02c</v>
       </c>
       <c r="E5">
-        <f>VLOOKUP(C5,Colors!A:C,3,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D5,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <f>VLOOKUP(E5,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -1202,11 +1224,15 @@
         <v>#33a02c</v>
       </c>
       <c r="E6">
-        <f>VLOOKUP(C6,Colors!A:C,3,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D6,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <f>VLOOKUP(E6,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1221,11 +1247,15 @@
         <v>#33a02c</v>
       </c>
       <c r="E7">
-        <f>VLOOKUP(C7,Colors!A:C,3,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D7,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <f>VLOOKUP(E7,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1240,11 +1270,15 @@
         <v>#33a02c</v>
       </c>
       <c r="E8">
-        <f>VLOOKUP(C8,Colors!A:C,3,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D8,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <f>VLOOKUP(E8,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1259,11 +1293,15 @@
         <v>#33a02c</v>
       </c>
       <c r="E9">
-        <f>VLOOKUP(C9,Colors!A:C,3,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D9,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <f>VLOOKUP(E9,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1278,11 +1316,15 @@
         <v>#33a02c</v>
       </c>
       <c r="E10">
-        <f>VLOOKUP(C10,Colors!A:C,3,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D10,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <f>VLOOKUP(E10,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -1297,11 +1339,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E11">
-        <f>VLOOKUP(C11,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D11,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <f>VLOOKUP(E11,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1316,11 +1362,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E12">
-        <f>VLOOKUP(C12,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D12,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <f>VLOOKUP(E12,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1335,11 +1385,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E13">
-        <f>VLOOKUP(C13,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D13,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <f>VLOOKUP(E13,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1354,11 +1408,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E14">
-        <f>VLOOKUP(C14,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D14,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <f>VLOOKUP(E14,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1373,11 +1431,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E15">
-        <f>VLOOKUP(C15,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D15,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <f>VLOOKUP(E15,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1392,11 +1454,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E16">
-        <f>VLOOKUP(C16,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D16,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <f>VLOOKUP(E16,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>159</v>
       </c>
@@ -1411,11 +1477,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E17">
-        <f>VLOOKUP(C17,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D17,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <f>VLOOKUP(E17,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>161</v>
       </c>
@@ -1430,11 +1500,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E18">
-        <f>VLOOKUP(C18,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D18,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <f>VLOOKUP(E18,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -1449,11 +1523,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E19">
-        <f>VLOOKUP(C19,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D19,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <f>VLOOKUP(E19,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>173</v>
       </c>
@@ -1468,11 +1546,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E20">
-        <f>VLOOKUP(C20,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D20,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <f>VLOOKUP(E20,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>175</v>
       </c>
@@ -1487,11 +1569,15 @@
         <v>#fb9a99</v>
       </c>
       <c r="E21">
-        <f>VLOOKUP(C21,Colors!A:C,3,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D21,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <f>VLOOKUP(E21,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -1506,11 +1592,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E22">
-        <f>VLOOKUP(C22,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D22,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <f>VLOOKUP(E22,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>139</v>
       </c>
@@ -1525,11 +1615,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E23">
-        <f>VLOOKUP(C23,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D23,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <f>VLOOKUP(E23,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>141</v>
       </c>
@@ -1544,11 +1638,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E24">
-        <f>VLOOKUP(C24,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D24,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <f>VLOOKUP(E24,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -1563,11 +1661,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E25">
-        <f>VLOOKUP(C25,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D25,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <f>VLOOKUP(E25,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -1582,11 +1684,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E26">
-        <f>VLOOKUP(C26,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D26,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <f>VLOOKUP(E26,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>152</v>
       </c>
@@ -1601,11 +1707,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E27">
-        <f>VLOOKUP(C27,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D27,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <f>VLOOKUP(E27,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -1620,11 +1730,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E28">
-        <f>VLOOKUP(C28,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D28,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <f>VLOOKUP(E28,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1639,11 +1753,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E29">
-        <f>VLOOKUP(C29,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D29,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F29">
+        <f>VLOOKUP(E29,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1658,11 +1776,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E30">
-        <f>VLOOKUP(C30,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D30,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <f>VLOOKUP(E30,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -1677,11 +1799,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E31">
-        <f>VLOOKUP(C31,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D31,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <f>VLOOKUP(E31,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>169</v>
       </c>
@@ -1696,11 +1822,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E32">
-        <f>VLOOKUP(C32,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D32,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <f>VLOOKUP(E32,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>171</v>
       </c>
@@ -1715,11 +1845,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E33">
-        <f>VLOOKUP(C33,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D33,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F33">
+        <f>VLOOKUP(E33,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>179</v>
       </c>
@@ -1734,11 +1868,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E34">
-        <f>VLOOKUP(C34,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D34,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F34">
+        <f>VLOOKUP(E34,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -1753,11 +1891,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E35">
-        <f>VLOOKUP(C35,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D35,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <f>VLOOKUP(E35,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>182</v>
       </c>
@@ -1772,11 +1914,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E36">
-        <f>VLOOKUP(C36,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D36,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <f>VLOOKUP(E36,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>184</v>
       </c>
@@ -1791,11 +1937,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E37">
-        <f>VLOOKUP(C37,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D37,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F37">
+        <f>VLOOKUP(E37,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>186</v>
       </c>
@@ -1810,11 +1960,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E38">
-        <f>VLOOKUP(C38,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D38,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F38">
+        <f>VLOOKUP(E38,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>188</v>
       </c>
@@ -1829,11 +1983,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E39">
-        <f>VLOOKUP(C39,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D39,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F39">
+        <f>VLOOKUP(E39,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -1848,11 +2006,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E40">
-        <f>VLOOKUP(C40,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D40,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F40">
+        <f>VLOOKUP(E40,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>218</v>
       </c>
@@ -1867,11 +2029,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E41">
-        <f>VLOOKUP(C41,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D41,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F41">
+        <f>VLOOKUP(E41,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>224</v>
       </c>
@@ -1886,11 +2052,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E42">
-        <f>VLOOKUP(C42,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D42,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <f>VLOOKUP(E42,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>225</v>
       </c>
@@ -1905,11 +2075,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E43">
-        <f>VLOOKUP(C43,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D43,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F43">
+        <f>VLOOKUP(E43,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>222</v>
       </c>
@@ -1924,11 +2098,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E44">
-        <f>VLOOKUP(C44,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D44,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F44">
+        <f>VLOOKUP(E44,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>223</v>
       </c>
@@ -1943,11 +2121,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E45">
-        <f>VLOOKUP(C45,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D45,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F45">
+        <f>VLOOKUP(E45,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>206</v>
       </c>
@@ -1962,11 +2144,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E46">
-        <f>VLOOKUP(C46,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D46,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F46">
+        <f>VLOOKUP(E46,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>235</v>
       </c>
@@ -1981,11 +2167,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E47">
-        <f>VLOOKUP(C47,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D47,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F47">
+        <f>VLOOKUP(E47,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>213</v>
       </c>
@@ -2000,11 +2190,15 @@
         <v>#cab2d6</v>
       </c>
       <c r="E48">
-        <f>VLOOKUP(C48,Colors!A:C,3,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D48,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F48">
+        <f>VLOOKUP(E48,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -2019,11 +2213,15 @@
         <v>#fdbf6f</v>
       </c>
       <c r="E49">
-        <f>VLOOKUP(C49,Colors!A:C,3,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D49,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F49">
+        <f>VLOOKUP(E49,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2038,11 +2236,15 @@
         <v>#fdbf6f</v>
       </c>
       <c r="E50">
-        <f>VLOOKUP(C50,Colors!A:C,3,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D50,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F50">
+        <f>VLOOKUP(E50,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>234</v>
       </c>
@@ -2057,11 +2259,15 @@
         <v>#fdbf6f</v>
       </c>
       <c r="E51">
-        <f>VLOOKUP(C51,Colors!A:C,3,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D51,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F51">
+        <f>VLOOKUP(E51,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>214</v>
       </c>
@@ -2076,11 +2282,15 @@
         <v>#fdbf6f</v>
       </c>
       <c r="E52">
-        <f>VLOOKUP(C52,Colors!A:C,3,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D52,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F52">
+        <f>VLOOKUP(E52,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>230</v>
       </c>
@@ -2095,11 +2305,15 @@
         <v>#fdbf6f</v>
       </c>
       <c r="E53">
-        <f>VLOOKUP(C53,Colors!A:C,3,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D53,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F53">
+        <f>VLOOKUP(E53,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>229</v>
       </c>
@@ -2114,11 +2328,15 @@
         <v>#fdbf6f</v>
       </c>
       <c r="E54">
-        <f>VLOOKUP(C54,Colors!A:C,3,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D54,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F54">
+        <f>VLOOKUP(E54,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>226</v>
       </c>
@@ -2133,11 +2351,15 @@
         <v>#fdbf6f</v>
       </c>
       <c r="E55">
-        <f>VLOOKUP(C55,Colors!A:C,3,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D55,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F55">
+        <f>VLOOKUP(E55,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>227</v>
       </c>
@@ -2152,11 +2374,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E56">
-        <f>VLOOKUP(C56,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D56,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F56">
+        <f>VLOOKUP(E56,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>157</v>
       </c>
@@ -2171,11 +2397,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E57">
-        <f>VLOOKUP(C57,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D57,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F57">
+        <f>VLOOKUP(E57,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -2190,11 +2420,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E58">
-        <f>VLOOKUP(C58,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D58,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F58">
+        <f>VLOOKUP(E58,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -2209,11 +2443,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E59">
-        <f>VLOOKUP(C59,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D59,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F59">
+        <f>VLOOKUP(E59,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -2228,11 +2466,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E60">
-        <f>VLOOKUP(C60,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D60,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F60">
+        <f>VLOOKUP(E60,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -2247,11 +2489,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E61">
-        <f>VLOOKUP(C61,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D61,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F61">
+        <f>VLOOKUP(E61,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>165</v>
       </c>
@@ -2266,11 +2512,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E62">
-        <f>VLOOKUP(C62,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D62,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F62">
+        <f>VLOOKUP(E62,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>233</v>
       </c>
@@ -2285,11 +2535,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E63">
-        <f>VLOOKUP(C63,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D63,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F63">
+        <f>VLOOKUP(E63,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>221</v>
       </c>
@@ -2304,11 +2558,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E64">
-        <f>VLOOKUP(C64,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D64,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F64">
+        <f>VLOOKUP(E64,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>228</v>
       </c>
@@ -2323,11 +2581,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E65">
-        <f>VLOOKUP(C65,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D65,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F65">
+        <f>VLOOKUP(E65,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>217</v>
       </c>
@@ -2342,11 +2604,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E66">
-        <f>VLOOKUP(C66,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D66,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F66">
+        <f>VLOOKUP(E66,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>220</v>
       </c>
@@ -2361,11 +2627,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E67">
-        <f>VLOOKUP(C67,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D67,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F67">
+        <f>VLOOKUP(E67,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>232</v>
       </c>
@@ -2380,11 +2650,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E68">
-        <f>VLOOKUP(C68,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D68,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F68">
+        <f>VLOOKUP(E68,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>231</v>
       </c>
@@ -2399,11 +2673,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E69">
-        <f>VLOOKUP(C69,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D69,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F69">
+        <f>VLOOKUP(E69,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>219</v>
       </c>
@@ -2418,11 +2696,15 @@
         <v>#e31a1c</v>
       </c>
       <c r="E70">
-        <f>VLOOKUP(C70,Colors!A:C,3,FALSE)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D70,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F70">
+        <f>VLOOKUP(E70,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>51</v>
       </c>
@@ -2437,11 +2719,15 @@
         <v>#6a3d9a</v>
       </c>
       <c r="E71">
-        <f>VLOOKUP(C71,Colors!A:C,3,FALSE)</f>
+        <f>VLOOKUP(D71,Colors!B:C,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F71">
+        <f>VLOOKUP(E71,Colors!C:D,2,FALSE)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -2456,11 +2742,15 @@
         <v>#b2df8a</v>
       </c>
       <c r="E72">
-        <f>VLOOKUP(C72,Colors!A:C,3,FALSE)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D72,Colors!B:C,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F72">
+        <f>VLOOKUP(E72,Colors!C:D,2,FALSE)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -2475,11 +2765,15 @@
         <v>#ff7f00</v>
       </c>
       <c r="E73">
-        <f>VLOOKUP(C73,Colors!A:C,3,FALSE)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D73,Colors!B:C,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F73">
+        <f>VLOOKUP(E73,Colors!C:D,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -2494,11 +2788,15 @@
         <v>#1f78b4</v>
       </c>
       <c r="E74">
-        <f>VLOOKUP(C74,Colors!A:C,3,FALSE)</f>
+        <f>VLOOKUP(D74,Colors!B:C,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="F74">
+        <f>VLOOKUP(E74,Colors!C:D,2,FALSE)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>69</v>
       </c>
@@ -2513,11 +2811,15 @@
         <v>#b15928</v>
       </c>
       <c r="E75">
-        <f>VLOOKUP(C75,Colors!A:C,3,FALSE)</f>
+        <f>VLOOKUP(D75,Colors!B:C,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="F75">
+        <f>VLOOKUP(E75,Colors!C:D,2,FALSE)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>72</v>
       </c>
@@ -2532,11 +2834,15 @@
         <v>#003c30</v>
       </c>
       <c r="E76">
-        <f>VLOOKUP(C76,Colors!A:C,3,FALSE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D76,Colors!B:C,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="F76">
+        <f>VLOOKUP(E76,Colors!C:D,2,FALSE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2551,11 +2857,15 @@
         <v>#003c30</v>
       </c>
       <c r="E77">
-        <f>VLOOKUP(C77,Colors!A:C,3,FALSE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D77,Colors!B:C,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="F77">
+        <f>VLOOKUP(E77,Colors!C:D,2,FALSE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2570,11 +2880,15 @@
         <v>#003c30</v>
       </c>
       <c r="E78">
-        <f>VLOOKUP(C78,Colors!A:C,3,FALSE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D78,Colors!B:C,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="F78">
+        <f>VLOOKUP(E78,Colors!C:D,2,FALSE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>177</v>
       </c>
@@ -2589,11 +2903,15 @@
         <v>#4d4d4d</v>
       </c>
       <c r="E79">
-        <f>VLOOKUP(C79,Colors!A:C,3,FALSE)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <f>VLOOKUP(D79,Colors!B:C,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="F79">
+        <f>VLOOKUP(E79,Colors!C:D,2,FALSE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>66</v>
       </c>
@@ -2608,18 +2926,22 @@
         <v>#ae017e</v>
       </c>
       <c r="E80">
-        <f>VLOOKUP(C80,Colors!A:C,3,FALSE)</f>
-        <v>14</v>
+        <f>VLOOKUP(D80,Colors!B:C,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="F80">
+        <f>VLOOKUP(E80,Colors!C:D,2,FALSE)</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E29">
-    <sortState ref="A2:E80">
-      <sortCondition ref="E1:E80"/>
+  <autoFilter ref="A1:F29">
+    <sortState ref="A2:F80">
+      <sortCondition ref="F1:F80"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:E80">
-    <sortCondition ref="E2:E80"/>
+  <sortState ref="A2:F80">
+    <sortCondition ref="F2:F80"/>
     <sortCondition ref="A2:A80"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2629,10 +2951,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2640,7 +2962,7 @@
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2648,10 +2970,13 @@
         <v>7</v>
       </c>
       <c r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2659,10 +2984,13 @@
         <v>17</v>
       </c>
       <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2670,10 +2998,13 @@
         <v>21</v>
       </c>
       <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2681,10 +3012,13 @@
         <v>48</v>
       </c>
       <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2692,10 +3026,13 @@
         <v>37</v>
       </c>
       <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2703,10 +3040,13 @@
         <v>25</v>
       </c>
       <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2714,10 +3054,13 @@
         <v>53</v>
       </c>
       <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2725,10 +3068,13 @@
         <v>13</v>
       </c>
       <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2736,10 +3082,13 @@
         <v>40</v>
       </c>
       <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2747,10 +3096,13 @@
         <v>11</v>
       </c>
       <c r="C10">
+        <v>18</v>
+      </c>
+      <c r="D10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2758,10 +3110,13 @@
         <v>71</v>
       </c>
       <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -2769,10 +3124,13 @@
         <v>75</v>
       </c>
       <c r="C12">
+        <v>17</v>
+      </c>
+      <c r="D12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>132</v>
       </c>
@@ -2780,10 +3138,13 @@
         <v>81</v>
       </c>
       <c r="C13">
+        <v>17</v>
+      </c>
+      <c r="D13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -2791,6 +3152,9 @@
         <v>133</v>
       </c>
       <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
name changes and meta pop ordering
</commit_message>
<xml_diff>
--- a/pop_names.xlsx
+++ b/pop_names.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="238">
   <si>
     <t>Code</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Coyote</t>
   </si>
   <si>
-    <t>Coyotes</t>
-  </si>
-  <si>
     <t>#1f78b4</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Alaskan Husky</t>
   </si>
   <si>
-    <t>Northern Dogs</t>
-  </si>
-  <si>
     <t>#fb9a99</t>
   </si>
   <si>
@@ -750,6 +744,9 @@
   </si>
   <si>
     <t>Shape</t>
+  </si>
+  <si>
+    <t>Arctic Dogs</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1084,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1111,10 +1108,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1132,17 +1129,17 @@
         <v>#a6cee3</v>
       </c>
       <c r="E2">
-        <f>VLOOKUP(D2,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C2,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F2">
-        <f>VLOOKUP(E2,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C2,Colors!A:D,4,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1155,20 +1152,20 @@
         <v>#a6cee3</v>
       </c>
       <c r="E3">
-        <f>VLOOKUP(D3,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C3,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F3">
-        <f>VLOOKUP(E3,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C3,Colors!A:D,4,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1178,1667 +1175,1667 @@
         <v>#a6cee3</v>
       </c>
       <c r="E4">
-        <f>VLOOKUP(D4,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C4,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F4">
-        <f>VLOOKUP(E4,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C4,Colors!A:D,4,FALSE)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="str">
         <f>VLOOKUP(C5,Colors!A:B,2,FALSE)</f>
         <v>#33a02c</v>
       </c>
       <c r="E5">
-        <f>VLOOKUP(D5,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C5,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F5">
-        <f>VLOOKUP(E5,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C5,Colors!A:D,4,FALSE)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="str">
         <f>VLOOKUP(C6,Colors!A:B,2,FALSE)</f>
         <v>#33a02c</v>
       </c>
       <c r="E6">
-        <f>VLOOKUP(D6,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C6,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F6">
-        <f>VLOOKUP(E6,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C6,Colors!A:D,4,FALSE)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="str">
         <f>VLOOKUP(C7,Colors!A:B,2,FALSE)</f>
         <v>#33a02c</v>
       </c>
       <c r="E7">
-        <f>VLOOKUP(D7,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C7,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F7">
-        <f>VLOOKUP(E7,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C7,Colors!A:D,4,FALSE)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="str">
         <f>VLOOKUP(C8,Colors!A:B,2,FALSE)</f>
         <v>#33a02c</v>
       </c>
       <c r="E8">
-        <f>VLOOKUP(D8,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C8,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F8">
-        <f>VLOOKUP(E8,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C8,Colors!A:D,4,FALSE)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="str">
         <f>VLOOKUP(C9,Colors!A:B,2,FALSE)</f>
         <v>#33a02c</v>
       </c>
       <c r="E9">
-        <f>VLOOKUP(D9,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C9,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F9">
-        <f>VLOOKUP(E9,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C9,Colors!A:D,4,FALSE)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="str">
         <f>VLOOKUP(C10,Colors!A:B,2,FALSE)</f>
         <v>#33a02c</v>
       </c>
       <c r="E10">
-        <f>VLOOKUP(D10,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C10,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F10">
-        <f>VLOOKUP(E10,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C10,Colors!A:D,4,FALSE)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D11" t="str">
         <f>VLOOKUP(C11,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E11">
-        <f>VLOOKUP(D11,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C11,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F11">
-        <f>VLOOKUP(E11,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C11,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D12" t="str">
         <f>VLOOKUP(C12,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E12">
-        <f>VLOOKUP(D12,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C12,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F12">
-        <f>VLOOKUP(E12,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C12,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D13" t="str">
         <f>VLOOKUP(C13,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E13">
-        <f>VLOOKUP(D13,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C13,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F13">
-        <f>VLOOKUP(E13,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C13,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D14" t="str">
         <f>VLOOKUP(C14,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E14">
-        <f>VLOOKUP(D14,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C14,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F14">
-        <f>VLOOKUP(E14,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C14,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D15" t="str">
         <f>VLOOKUP(C15,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E15">
-        <f>VLOOKUP(D15,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C15,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F15">
-        <f>VLOOKUP(E15,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C15,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D16" t="str">
         <f>VLOOKUP(C16,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E16">
-        <f>VLOOKUP(D16,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C16,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F16">
-        <f>VLOOKUP(E16,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C16,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D17" t="str">
         <f>VLOOKUP(C17,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E17">
-        <f>VLOOKUP(D17,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C17,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F17">
-        <f>VLOOKUP(E17,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C17,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D18" t="str">
         <f>VLOOKUP(C18,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E18">
-        <f>VLOOKUP(D18,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C18,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F18">
-        <f>VLOOKUP(E18,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C18,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D19" t="str">
         <f>VLOOKUP(C19,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E19">
-        <f>VLOOKUP(D19,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C19,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F19">
-        <f>VLOOKUP(E19,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C19,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D20" t="str">
         <f>VLOOKUP(C20,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E20">
-        <f>VLOOKUP(D20,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C20,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F20">
-        <f>VLOOKUP(E20,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C20,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D21" t="str">
         <f>VLOOKUP(C21,Colors!A:B,2,FALSE)</f>
         <v>#fb9a99</v>
       </c>
       <c r="E21">
-        <f>VLOOKUP(D21,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C21,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F21">
-        <f>VLOOKUP(E21,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C21,Colors!A:D,4,FALSE)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" t="str">
         <f>VLOOKUP(C22,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E22">
-        <f>VLOOKUP(D22,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C22,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F22">
-        <f>VLOOKUP(E22,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C22,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23" t="str">
         <f>VLOOKUP(C23,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E23">
-        <f>VLOOKUP(D23,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C23,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F23">
-        <f>VLOOKUP(E23,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C23,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" t="str">
         <f>VLOOKUP(C24,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E24">
-        <f>VLOOKUP(D24,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C24,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F24">
-        <f>VLOOKUP(E24,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C24,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" t="str">
         <f>VLOOKUP(C25,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E25">
-        <f>VLOOKUP(D25,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C25,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F25">
-        <f>VLOOKUP(E25,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C25,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D26" t="str">
         <f>VLOOKUP(C26,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E26">
-        <f>VLOOKUP(D26,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C26,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F26">
-        <f>VLOOKUP(E26,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C26,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" t="str">
         <f>VLOOKUP(C27,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E27">
-        <f>VLOOKUP(D27,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C27,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F27">
-        <f>VLOOKUP(E27,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C27,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28" t="str">
         <f>VLOOKUP(C28,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E28">
-        <f>VLOOKUP(D28,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C28,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F28">
-        <f>VLOOKUP(E28,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C28,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
         <v>45</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" t="s">
-        <v>47</v>
       </c>
       <c r="D29" t="str">
         <f>VLOOKUP(C29,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E29">
-        <f>VLOOKUP(D29,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C29,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F29">
-        <f>VLOOKUP(E29,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C29,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30" t="str">
         <f>VLOOKUP(C30,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E30">
-        <f>VLOOKUP(D30,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C30,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F30">
-        <f>VLOOKUP(E30,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C30,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D31" t="str">
         <f>VLOOKUP(C31,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E31">
-        <f>VLOOKUP(D31,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C31,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F31">
-        <f>VLOOKUP(E31,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C31,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D32" t="str">
         <f>VLOOKUP(C32,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E32">
-        <f>VLOOKUP(D32,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C32,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F32">
-        <f>VLOOKUP(E32,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C32,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" t="str">
         <f>VLOOKUP(C33,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E33">
-        <f>VLOOKUP(D33,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C33,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F33">
-        <f>VLOOKUP(E33,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C33,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D34" t="str">
         <f>VLOOKUP(C34,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E34">
-        <f>VLOOKUP(D34,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C34,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F34">
-        <f>VLOOKUP(E34,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C34,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D35" t="str">
         <f>VLOOKUP(C35,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E35">
-        <f>VLOOKUP(D35,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C35,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F35">
-        <f>VLOOKUP(E35,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C35,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D36" t="str">
         <f>VLOOKUP(C36,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E36">
-        <f>VLOOKUP(D36,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C36,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F36">
-        <f>VLOOKUP(E36,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C36,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" t="str">
         <f>VLOOKUP(C37,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E37">
-        <f>VLOOKUP(D37,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C37,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F37">
-        <f>VLOOKUP(E37,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C37,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D38" t="str">
         <f>VLOOKUP(C38,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E38">
-        <f>VLOOKUP(D38,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C38,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F38">
-        <f>VLOOKUP(E38,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C38,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D39" t="str">
         <f>VLOOKUP(C39,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E39">
-        <f>VLOOKUP(D39,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C39,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F39">
-        <f>VLOOKUP(E39,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C39,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D40" t="str">
         <f>VLOOKUP(C40,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E40">
-        <f>VLOOKUP(D40,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C40,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F40">
-        <f>VLOOKUP(E40,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C40,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D41" t="str">
         <f>VLOOKUP(C41,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E41">
-        <f>VLOOKUP(D41,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C41,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F41">
-        <f>VLOOKUP(E41,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C41,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D42" t="str">
         <f>VLOOKUP(C42,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E42">
-        <f>VLOOKUP(D42,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C42,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F42">
-        <f>VLOOKUP(E42,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C42,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D43" t="str">
         <f>VLOOKUP(C43,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E43">
-        <f>VLOOKUP(D43,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C43,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F43">
-        <f>VLOOKUP(E43,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C43,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D44" t="str">
         <f>VLOOKUP(C44,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E44">
-        <f>VLOOKUP(D44,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C44,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F44">
-        <f>VLOOKUP(E44,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C44,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D45" t="str">
         <f>VLOOKUP(C45,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E45">
-        <f>VLOOKUP(D45,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C45,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F45">
-        <f>VLOOKUP(E45,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C45,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D46" t="str">
         <f>VLOOKUP(C46,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E46">
-        <f>VLOOKUP(D46,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C46,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F46">
-        <f>VLOOKUP(E46,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C46,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D47" t="str">
         <f>VLOOKUP(C47,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E47">
-        <f>VLOOKUP(D47,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C47,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F47">
-        <f>VLOOKUP(E47,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C47,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D48" t="str">
         <f>VLOOKUP(C48,Colors!A:B,2,FALSE)</f>
         <v>#cab2d6</v>
       </c>
       <c r="E48">
-        <f>VLOOKUP(D48,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C48,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F48">
-        <f>VLOOKUP(E48,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C48,Colors!A:D,4,FALSE)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" t="s">
         <v>34</v>
-      </c>
-      <c r="B49" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" t="s">
-        <v>36</v>
       </c>
       <c r="D49" t="str">
         <f>VLOOKUP(C49,Colors!A:B,2,FALSE)</f>
         <v>#fdbf6f</v>
       </c>
       <c r="E49">
-        <f>VLOOKUP(D49,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C49,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F49">
-        <f>VLOOKUP(E49,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C49,Colors!A:D,4,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D50" t="str">
         <f>VLOOKUP(C50,Colors!A:B,2,FALSE)</f>
         <v>#fdbf6f</v>
       </c>
       <c r="E50">
-        <f>VLOOKUP(D50,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C50,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F50">
-        <f>VLOOKUP(E50,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C50,Colors!A:D,4,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D51" t="str">
         <f>VLOOKUP(C51,Colors!A:B,2,FALSE)</f>
         <v>#fdbf6f</v>
       </c>
       <c r="E51">
-        <f>VLOOKUP(D51,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C51,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F51">
-        <f>VLOOKUP(E51,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C51,Colors!A:D,4,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D52" t="str">
         <f>VLOOKUP(C52,Colors!A:B,2,FALSE)</f>
         <v>#fdbf6f</v>
       </c>
       <c r="E52">
-        <f>VLOOKUP(D52,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C52,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F52">
-        <f>VLOOKUP(E52,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C52,Colors!A:D,4,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D53" t="str">
         <f>VLOOKUP(C53,Colors!A:B,2,FALSE)</f>
         <v>#fdbf6f</v>
       </c>
       <c r="E53">
-        <f>VLOOKUP(D53,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C53,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F53">
-        <f>VLOOKUP(E53,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C53,Colors!A:D,4,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D54" t="str">
         <f>VLOOKUP(C54,Colors!A:B,2,FALSE)</f>
         <v>#fdbf6f</v>
       </c>
       <c r="E54">
-        <f>VLOOKUP(D54,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C54,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F54">
-        <f>VLOOKUP(E54,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C54,Colors!A:D,4,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D55" t="str">
         <f>VLOOKUP(C55,Colors!A:B,2,FALSE)</f>
         <v>#fdbf6f</v>
       </c>
       <c r="E55">
-        <f>VLOOKUP(D55,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C55,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F55">
-        <f>VLOOKUP(E55,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C55,Colors!A:D,4,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D56" t="str">
         <f>VLOOKUP(C56,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E56">
-        <f>VLOOKUP(D56,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C56,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F56">
-        <f>VLOOKUP(E56,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C56,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D57" t="str">
         <f>VLOOKUP(C57,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E57">
-        <f>VLOOKUP(D57,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C57,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F57">
-        <f>VLOOKUP(E57,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C57,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" t="s">
         <v>22</v>
-      </c>
-      <c r="B58" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58" t="s">
-        <v>24</v>
       </c>
       <c r="D58" t="str">
         <f>VLOOKUP(C58,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E58">
-        <f>VLOOKUP(D58,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C58,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F58">
-        <f>VLOOKUP(E58,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C58,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D59" t="str">
         <f>VLOOKUP(C59,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E59">
-        <f>VLOOKUP(D59,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C59,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F59">
-        <f>VLOOKUP(E59,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C59,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D60" t="str">
         <f>VLOOKUP(C60,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E60">
-        <f>VLOOKUP(D60,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C60,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F60">
-        <f>VLOOKUP(E60,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C60,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D61" t="str">
         <f>VLOOKUP(C61,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E61">
-        <f>VLOOKUP(D61,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C61,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F61">
-        <f>VLOOKUP(E61,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C61,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D62" t="str">
         <f>VLOOKUP(C62,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E62">
-        <f>VLOOKUP(D62,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C62,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F62">
-        <f>VLOOKUP(E62,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C62,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B63" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D63" t="str">
         <f>VLOOKUP(C63,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E63">
-        <f>VLOOKUP(D63,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C63,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F63">
-        <f>VLOOKUP(E63,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C63,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D64" t="str">
         <f>VLOOKUP(C64,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E64">
-        <f>VLOOKUP(D64,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C64,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F64">
-        <f>VLOOKUP(E64,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C64,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D65" t="str">
         <f>VLOOKUP(C65,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E65">
-        <f>VLOOKUP(D65,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C65,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F65">
-        <f>VLOOKUP(E65,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C65,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D66" t="str">
         <f>VLOOKUP(C66,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E66">
-        <f>VLOOKUP(D66,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C66,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F66">
-        <f>VLOOKUP(E66,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C66,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C67" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D67" t="str">
         <f>VLOOKUP(C67,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E67">
-        <f>VLOOKUP(D67,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C67,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F67">
-        <f>VLOOKUP(E67,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C67,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C68" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D68" t="str">
         <f>VLOOKUP(C68,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E68">
-        <f>VLOOKUP(D68,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C68,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F68">
-        <f>VLOOKUP(E68,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C68,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C69" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D69" t="str">
         <f>VLOOKUP(C69,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E69">
-        <f>VLOOKUP(D69,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C69,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F69">
-        <f>VLOOKUP(E69,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C69,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B70" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C70" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D70" t="str">
         <f>VLOOKUP(C70,Colors!A:B,2,FALSE)</f>
         <v>#e31a1c</v>
       </c>
       <c r="E70">
-        <f>VLOOKUP(D70,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C70,Colors!A:C,3,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F70">
-        <f>VLOOKUP(E70,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C70,Colors!A:D,4,FALSE)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B71" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D71" t="str">
         <f>VLOOKUP(C71,Colors!A:B,2,FALSE)</f>
-        <v>#6a3d9a</v>
+        <v>#ff7f00</v>
       </c>
       <c r="E71">
-        <f>VLOOKUP(D71,Colors!B:C,2,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C71,Colors!A:C,3,FALSE)</f>
+        <v>15</v>
       </c>
       <c r="F71">
-        <f>VLOOKUP(E71,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C71,Colors!A:D,4,FALSE)</f>
         <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C72" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D72" t="str">
         <f>VLOOKUP(C72,Colors!A:B,2,FALSE)</f>
-        <v>#b2df8a</v>
+        <v>#6a3d9a</v>
       </c>
       <c r="E72">
-        <f>VLOOKUP(D72,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C72,Colors!A:C,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F72">
-        <f>VLOOKUP(E72,Colors!C:D,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(C72,Colors!A:D,4,FALSE)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D73" t="str">
         <f>VLOOKUP(C73,Colors!A:B,2,FALSE)</f>
-        <v>#ff7f00</v>
+        <v>#b2df8a</v>
       </c>
       <c r="E73">
-        <f>VLOOKUP(D73,Colors!B:C,2,FALSE)</f>
-        <v>15</v>
+        <f>VLOOKUP(C73,Colors!A:C,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F73">
-        <f>VLOOKUP(E73,Colors!C:D,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(C73,Colors!A:D,4,FALSE)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D74" t="str">
         <f>VLOOKUP(C74,Colors!A:B,2,FALSE)</f>
-        <v>#1f78b4</v>
+        <v>#b15928</v>
       </c>
       <c r="E74">
-        <f>VLOOKUP(D74,Colors!B:C,2,FALSE)</f>
-        <v>18</v>
+        <f>VLOOKUP(C74,Colors!A:C,3,FALSE)</f>
+        <v>17</v>
       </c>
       <c r="F74">
-        <f>VLOOKUP(E74,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C74,Colors!A:D,4,FALSE)</f>
         <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D75" t="str">
         <f>VLOOKUP(C75,Colors!A:B,2,FALSE)</f>
-        <v>#b15928</v>
+        <v>#003c30</v>
       </c>
       <c r="E75">
-        <f>VLOOKUP(D75,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C75,Colors!A:C,3,FALSE)</f>
         <v>17</v>
       </c>
       <c r="F75">
-        <f>VLOOKUP(E75,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C75,Colors!A:D,4,FALSE)</f>
         <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" t="s">
         <v>72</v>
-      </c>
-      <c r="B76" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" t="s">
-        <v>74</v>
       </c>
       <c r="D76" t="str">
         <f>VLOOKUP(C76,Colors!A:B,2,FALSE)</f>
         <v>#003c30</v>
       </c>
       <c r="E76">
-        <f>VLOOKUP(D76,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C76,Colors!A:C,3,FALSE)</f>
         <v>17</v>
       </c>
       <c r="F76">
-        <f>VLOOKUP(E76,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C76,Colors!A:D,4,FALSE)</f>
         <v>11</v>
       </c>
     </row>
@@ -2850,88 +2847,88 @@
         <v>77</v>
       </c>
       <c r="C77" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D77" t="str">
         <f>VLOOKUP(C77,Colors!A:B,2,FALSE)</f>
         <v>#003c30</v>
       </c>
       <c r="E77">
-        <f>VLOOKUP(D77,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C77,Colors!A:C,3,FALSE)</f>
         <v>17</v>
       </c>
       <c r="F77">
-        <f>VLOOKUP(E77,Colors!C:D,2,FALSE)</f>
+        <f>VLOOKUP(C77,Colors!A:D,4,FALSE)</f>
         <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="C78" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="D78" t="str">
         <f>VLOOKUP(C78,Colors!A:B,2,FALSE)</f>
-        <v>#003c30</v>
+        <v>#4d4d4d</v>
       </c>
       <c r="E78">
-        <f>VLOOKUP(D78,Colors!B:C,2,FALSE)</f>
-        <v>17</v>
+        <f>VLOOKUP(C78,Colors!A:C,3,FALSE)</f>
+        <v>18</v>
       </c>
       <c r="F78">
-        <f>VLOOKUP(E78,Colors!C:D,2,FALSE)</f>
-        <v>11</v>
+        <f>VLOOKUP(C78,Colors!A:D,4,FALSE)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
       <c r="D79" t="str">
         <f>VLOOKUP(C79,Colors!A:B,2,FALSE)</f>
-        <v>#4d4d4d</v>
+        <v>#1f78b4</v>
       </c>
       <c r="E79">
-        <f>VLOOKUP(D79,Colors!B:C,2,FALSE)</f>
-        <v>17</v>
+        <f>VLOOKUP(C79,Colors!A:C,3,FALSE)</f>
+        <v>18</v>
       </c>
       <c r="F79">
-        <f>VLOOKUP(E79,Colors!C:D,2,FALSE)</f>
-        <v>11</v>
+        <f>VLOOKUP(C79,Colors!A:D,4,FALSE)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" t="s">
         <v>66</v>
-      </c>
-      <c r="B80" t="s">
-        <v>67</v>
-      </c>
-      <c r="C80" t="s">
-        <v>68</v>
       </c>
       <c r="D80" t="str">
         <f>VLOOKUP(C80,Colors!A:B,2,FALSE)</f>
         <v>#ae017e</v>
       </c>
       <c r="E80">
-        <f>VLOOKUP(D80,Colors!B:C,2,FALSE)</f>
+        <f>VLOOKUP(C80,Colors!A:C,3,FALSE)</f>
         <v>18</v>
       </c>
       <c r="F80">
-        <f>VLOOKUP(E80,Colors!C:D,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(C80,Colors!A:D,4,FALSE)</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2954,7 +2951,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2978,10 +2975,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -2992,10 +2989,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -3006,10 +3003,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -3020,10 +3017,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -3034,10 +3031,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -3048,13 +3045,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -3062,10 +3059,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -3076,13 +3073,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>9</v>
@@ -3090,13 +3087,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -3104,10 +3101,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C11">
         <v>17</v>
@@ -3118,13 +3115,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -3132,13 +3129,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>13</v>
@@ -3146,10 +3143,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C14">
         <v>18</v>
@@ -3179,418 +3176,418 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B31" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B36" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B41" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B42" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B43" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B47" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B49" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B51" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B52" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
standardised pluralisation of names
</commit_message>
<xml_diff>
--- a/pop_names.xlsx
+++ b/pop_names.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="241">
   <si>
     <t>Code</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Asian Wolf</t>
   </si>
   <si>
-    <t>Eurasian Wolf</t>
-  </si>
-  <si>
     <t>#003c30</t>
   </si>
   <si>
@@ -422,9 +419,6 @@
     <t>Taimyr</t>
   </si>
   <si>
-    <t>Ancient Wolf</t>
-  </si>
-  <si>
     <t>#ae017e</t>
   </si>
   <si>
@@ -747,6 +741,21 @@
   </si>
   <si>
     <t>Pre-contact Dogs</t>
+  </si>
+  <si>
+    <t>American Wolves</t>
+  </si>
+  <si>
+    <t>Eurasian Wolves</t>
+  </si>
+  <si>
+    <t>Ancient Wolves</t>
+  </si>
+  <si>
+    <t>Coyotes</t>
+  </si>
+  <si>
+    <t>Dingos</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1097,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1112,10 +1121,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1143,7 +1152,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1189,10 +1198,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1212,10 +1221,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1327,13 +1336,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D11" t="str">
         <f>VLOOKUP(C11,Colors!A:B,2,FALSE)</f>
@@ -1356,7 +1365,7 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D12" t="str">
         <f>VLOOKUP(C12,Colors!A:B,2,FALSE)</f>
@@ -1379,7 +1388,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D13" t="str">
         <f>VLOOKUP(C13,Colors!A:B,2,FALSE)</f>
@@ -1402,7 +1411,7 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D14" t="str">
         <f>VLOOKUP(C14,Colors!A:B,2,FALSE)</f>
@@ -1425,7 +1434,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D15" t="str">
         <f>VLOOKUP(C15,Colors!A:B,2,FALSE)</f>
@@ -1448,7 +1457,7 @@
         <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D16" t="str">
         <f>VLOOKUP(C16,Colors!A:B,2,FALSE)</f>
@@ -1465,13 +1474,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D17" t="str">
         <f>VLOOKUP(C17,Colors!A:B,2,FALSE)</f>
@@ -1488,13 +1497,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D18" t="str">
         <f>VLOOKUP(C18,Colors!A:B,2,FALSE)</f>
@@ -1511,13 +1520,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D19" t="str">
         <f>VLOOKUP(C19,Colors!A:B,2,FALSE)</f>
@@ -1534,13 +1543,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D20" t="str">
         <f>VLOOKUP(C20,Colors!A:B,2,FALSE)</f>
@@ -1557,13 +1566,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D21" t="str">
         <f>VLOOKUP(C21,Colors!A:B,2,FALSE)</f>
@@ -1580,10 +1589,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
         <v>45</v>
@@ -1603,10 +1612,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
         <v>45</v>
@@ -1626,10 +1635,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
         <v>45</v>
@@ -1649,10 +1658,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
         <v>45</v>
@@ -1672,10 +1681,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
         <v>45</v>
@@ -1695,10 +1704,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -1718,10 +1727,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
         <v>45</v>
@@ -1787,10 +1796,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
         <v>45</v>
@@ -1810,10 +1819,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
         <v>45</v>
@@ -1833,10 +1842,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
         <v>45</v>
@@ -1856,10 +1865,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
         <v>45</v>
@@ -1879,10 +1888,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
         <v>45</v>
@@ -1902,10 +1911,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
         <v>45</v>
@@ -1925,10 +1934,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
         <v>45</v>
@@ -1948,10 +1957,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
         <v>45</v>
@@ -1971,10 +1980,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
         <v>45</v>
@@ -1994,10 +2003,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
@@ -2017,10 +2026,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
         <v>45</v>
@@ -2040,10 +2049,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C42" t="s">
         <v>45</v>
@@ -2063,10 +2072,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
         <v>45</v>
@@ -2086,10 +2095,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
@@ -2109,10 +2118,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
         <v>45</v>
@@ -2132,10 +2141,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C46" t="s">
         <v>45</v>
@@ -2155,10 +2164,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C47" t="s">
         <v>45</v>
@@ -2178,10 +2187,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
         <v>45</v>
@@ -2247,10 +2256,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
         <v>34</v>
@@ -2270,10 +2279,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
         <v>34</v>
@@ -2293,10 +2302,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C53" t="s">
         <v>34</v>
@@ -2316,10 +2325,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
         <v>34</v>
@@ -2339,10 +2348,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
         <v>34</v>
@@ -2362,10 +2371,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" t="s">
         <v>22</v>
@@ -2385,10 +2394,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" t="s">
         <v>22</v>
@@ -2500,10 +2509,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" t="s">
         <v>22</v>
@@ -2523,10 +2532,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C63" t="s">
         <v>22</v>
@@ -2546,10 +2555,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C64" t="s">
         <v>22</v>
@@ -2569,10 +2578,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C65" t="s">
         <v>22</v>
@@ -2592,10 +2601,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C66" t="s">
         <v>22</v>
@@ -2615,10 +2624,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C67" t="s">
         <v>22</v>
@@ -2638,10 +2647,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C68" t="s">
         <v>22</v>
@@ -2661,10 +2670,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C69" t="s">
         <v>22</v>
@@ -2684,10 +2693,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C70" t="s">
         <v>22</v>
@@ -2713,7 +2722,7 @@
         <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="D71" t="str">
         <f>VLOOKUP(C71,Colors!A:B,2,FALSE)</f>
@@ -2733,10 +2742,10 @@
         <v>49</v>
       </c>
       <c r="B72" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C72" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D72" t="str">
         <f>VLOOKUP(C72,Colors!A:B,2,FALSE)</f>
@@ -2782,7 +2791,7 @@
         <v>67</v>
       </c>
       <c r="C74" t="s">
-        <v>67</v>
+        <v>236</v>
       </c>
       <c r="D74" t="str">
         <f>VLOOKUP(C74,Colors!A:B,2,FALSE)</f>
@@ -2805,7 +2814,7 @@
         <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>71</v>
+        <v>237</v>
       </c>
       <c r="D75" t="str">
         <f>VLOOKUP(C75,Colors!A:B,2,FALSE)</f>
@@ -2822,13 +2831,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" t="s">
         <v>73</v>
       </c>
-      <c r="B76" t="s">
-        <v>74</v>
-      </c>
       <c r="C76" t="s">
-        <v>71</v>
+        <v>237</v>
       </c>
       <c r="D76" t="str">
         <f>VLOOKUP(C76,Colors!A:B,2,FALSE)</f>
@@ -2845,13 +2854,13 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
-        <v>76</v>
-      </c>
       <c r="C77" t="s">
-        <v>71</v>
+        <v>237</v>
       </c>
       <c r="D77" t="str">
         <f>VLOOKUP(C77,Colors!A:B,2,FALSE)</f>
@@ -2868,13 +2877,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
       <c r="D78" t="str">
         <f>VLOOKUP(C78,Colors!A:B,2,FALSE)</f>
@@ -2897,7 +2906,7 @@
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
+        <v>239</v>
       </c>
       <c r="D79" t="str">
         <f>VLOOKUP(C79,Colors!A:B,2,FALSE)</f>
@@ -2955,7 +2964,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2993,7 +3002,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -3049,7 +3058,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -3063,7 +3072,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -3091,7 +3100,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s">
         <v>68</v>
@@ -3105,10 +3114,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B11" t="s">
         <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
       </c>
       <c r="C11">
         <v>17</v>
@@ -3119,10 +3128,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12">
         <v>18</v>
@@ -3133,7 +3142,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>239</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3150,7 +3159,7 @@
         <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C14">
         <v>18</v>
@@ -3181,418 +3190,418 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B34" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B40" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B44" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B45" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B46" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B49" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B50" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>